<commit_message>
Background configuration along with source file in data section is updated
</commit_message>
<xml_diff>
--- a/data/source_file.xlsx
+++ b/data/source_file.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mukeshkr\Desktop\DefenseExtraction\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49602830-3181-4C11-9C3A-D2F13F2E3F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F704E67-A7E0-4C36-A12A-C12FB09F42E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1789C02F-0F05-431D-B1D8-FBD75DE85A9F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Source URL</t>
   </si>
@@ -47,13 +47,10 @@
     <t>Contract Description</t>
   </si>
   <si>
-    <t>https://www.war.gov/News/Contracts/Contract/Article/3042310/</t>
+    <t>Northrop Grumman Systems Corp., Aerospace Systems, Melbourne, Florida, is awarded a $12,015,026 modification (P00036) to a previously awarded cost-plus-fixed-fee contract (N0001914C0036). This modification increases the ceiling to extend services and adds hours increasing the full-scale fatigue repair time to achieve the required simulated flight hours in support of E-2D Advanced Hawkeye aircraft development. Work will be performed in El Segundo, California (59%); Melbourne, Florida (35%); and Bethpage, New York (6%), and is expected to be completed in June 2023. No funds will be obligated at time of award. The Naval Air Systems Command, Patuxent River, Maryland, is the contracting activity.</t>
   </si>
   <si>
-    <t>Palantir USG Inc., Palo Alto, California, has been awarded a $53,899,333 firm-fixed-price modification (P000010) to previously awarded contract FA8806-21-C-0010 for Project Brown Heron Data-as-a-Service. The contract modification provides for a Data-as-a-Service platform that supports three mission areas to automatically ingest data across the Department of the Air Force that informs personnel decisions, planning and operations and space situational awareness and command and control. Work will be performed in Palo Alto, California, and is expected to be completed by March 31, 2023. Fiscal 2022 operations and maintenance funds in the amount of $16,000,000 will be obligated at the time of award. The total cumulative face value of the contract is $175,399,333. Space Systems Command, Los Angeles Air Force Base, El Segundo, California, is the contracting activity.</t>
-  </si>
-  <si>
-    <t>Sierra Nevada Corp., Sparks, Nevada, has been awarded a $33,997,595 firm-fixed-price and cost-reimbursement-no-fee order modification (P00003) to contract FA8509-20-F-0014, under Basic Contract FA8509-19-D-0001, for the MC-130J Airborne Mission Networking program low rate initial production. This order provides for the procurement of production kits, spares, interim contactor support and weapon system trainer support. Work will be performed in Centennial, Colorado, and is expected to be completed by Jan. 19, 2023. Fiscal 2022 U.S. Southern Command other procurement funds in the amount of $8,283,414; and fiscal 2022 Air Force other procurement funds in the amount of $25,714,181 are being obligated at the time of award. Air Force Life Cycle Management Center, Robins Air Force Base, Georgia, is the contracting activity. (Awarded May 13, 2022)</t>
+    <t>https://www.defense.gov/News/Contracts/Contract/Article/2644648/</t>
   </si>
 </sst>
 </file>
@@ -63,7 +60,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -97,6 +94,21 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -116,7 +128,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -124,19 +136,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="5" xr:uid="{00F41B89-8AB3-4DEC-B344-7FC2A8535877}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{59B0006E-8B6C-423D-8CA5-489B9B84501F}"/>
@@ -475,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C32A2EF0-6AE5-4C15-9CF0-4CEB2FFB30C8}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -499,26 +513,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>3</v>
+    <row r="2" spans="1:3" ht="90" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>44705</v>
+        <v>44350</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>44705</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>